<commit_message>
Rectification de code de config
</commit_message>
<xml_diff>
--- a/storage/30-04-2024/ENCAISSEMENT.xlsx
+++ b/storage/30-04-2024/ENCAISSEMENT.xlsx
@@ -518,13 +518,13 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>10614</v>
+        <v>237464.9</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>6351061.88</v>
+        <v>6721787.58</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>6151061.88</v>
+        <v>6521787.58</v>
       </c>
     </row>
     <row r="5">
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>407313.75</v>
+        <v>634164.65</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>10218287.19</v>
+        <v>10589012.89</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>10018287.19</v>
+        <v>10389012.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>